<commit_message>
los residuales están chistosos:)
</commit_message>
<xml_diff>
--- a/6. Oscilador Torsional/data/datos_act3.xlsx
+++ b/6. Oscilador Torsional/data/datos_act3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\Intermedio\6. Oscilador Torsional\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Intermedio\Oscilador\Intermedio\6. Oscilador Torsional\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD44D29A-74ED-4070-9732-32F76B294536}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7174E45B-A5ED-4CDD-9489-8EFA4BF9592B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3408" yWindow="3072" windowWidth="11160" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -367,19 +367,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,7 +393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -408,7 +408,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1.8</v>
       </c>
@@ -423,7 +423,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-1.6</v>
       </c>
@@ -438,7 +438,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-1.4</v>
       </c>
@@ -453,7 +453,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-1.2</v>
       </c>
@@ -468,7 +468,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-1</v>
       </c>
@@ -483,7 +483,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.8</v>
       </c>
@@ -498,7 +498,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-0.6</v>
       </c>
@@ -513,7 +513,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-0.4</v>
       </c>
@@ -528,7 +528,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-0.2</v>
       </c>
@@ -543,7 +543,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
@@ -557,7 +557,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.2</v>
       </c>
@@ -572,7 +572,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.4</v>
       </c>
@@ -587,7 +587,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.6</v>
       </c>
@@ -602,7 +602,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.8</v>
       </c>
@@ -617,7 +617,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -632,7 +632,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.2</v>
       </c>
@@ -647,13 +647,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.4</v>
       </c>
       <c r="B19">
-        <f>3.52-3.01</f>
-        <v>0.51000000000000023</v>
+        <v>0.71</v>
       </c>
       <c r="C19">
         <v>0.01</v>
@@ -662,7 +661,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.6</v>
       </c>
@@ -677,7 +676,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.8</v>
       </c>
@@ -692,7 +691,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>

</xml_diff>